<commit_message>
klart igen....med fixat exempel
</commit_message>
<xml_diff>
--- a/timediff_11.xlsx
+++ b/timediff_11.xlsx
@@ -61,14 +61,15 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="166" formatCode="hh:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="hh:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="yyyy/mm/dd"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -161,21 +162,21 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E:E"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="17.55"/>
   </cols>
@@ -187,13 +188,13 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="0" t="s">
@@ -224,16 +225,16 @@
       <c r="A2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E2" s="2" t="n">
+      <c r="B2" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E2" s="1" t="n">
         <v>0.470509259259259</v>
       </c>
       <c r="F2" s="0" t="n">
@@ -250,16 +251,16 @@
       <c r="A3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E3" s="2" t="n">
+      <c r="B3" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E3" s="1" t="n">
         <v>0.470543981481481</v>
       </c>
       <c r="F3" s="0" t="n">
@@ -276,16 +277,16 @@
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E4" s="2" t="n">
+      <c r="B4" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E4" s="1" t="n">
         <v>0.47056712962963</v>
       </c>
       <c r="F4" s="0" t="n">
@@ -302,16 +303,16 @@
       <c r="A5" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E5" s="2" t="n">
+      <c r="B5" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E5" s="1" t="n">
         <v>0.470590277777778</v>
       </c>
       <c r="F5" s="0" t="n">
@@ -328,16 +329,16 @@
       <c r="A6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E6" s="2" t="n">
+      <c r="B6" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E6" s="1" t="n">
         <v>0.470613425925926</v>
       </c>
       <c r="F6" s="0" t="n">
@@ -354,16 +355,16 @@
       <c r="A7" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E7" s="2" t="n">
+      <c r="B7" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E7" s="1" t="n">
         <v>0.470636574074074</v>
       </c>
       <c r="F7" s="0" t="n">
@@ -380,16 +381,16 @@
       <c r="A8" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C8" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E8" s="2" t="n">
+      <c r="B8" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E8" s="1" t="n">
         <v>0.470659722222222</v>
       </c>
       <c r="F8" s="0" t="n">
@@ -406,16 +407,16 @@
       <c r="A9" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C9" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E9" s="2" t="n">
+      <c r="B9" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E9" s="1" t="n">
         <v>0.47068287037037</v>
       </c>
       <c r="F9" s="0" t="n">
@@ -432,16 +433,16 @@
       <c r="A10" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C10" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E10" s="2" t="n">
+      <c r="B10" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E10" s="1" t="n">
         <v>0.470706018518519</v>
       </c>
       <c r="F10" s="0" t="n">
@@ -458,16 +459,16 @@
       <c r="A11" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C11" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D11" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E11" s="2" t="n">
+      <c r="B11" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E11" s="1" t="n">
         <v>0.470740740740741</v>
       </c>
       <c r="F11" s="0" t="n">
@@ -484,16 +485,16 @@
       <c r="A12" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C12" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D12" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E12" s="2" t="n">
+      <c r="B12" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E12" s="1" t="n">
         <v>0.470763888888889</v>
       </c>
       <c r="F12" s="0" t="n">
@@ -510,16 +511,16 @@
       <c r="A13" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C13" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D13" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E13" s="2" t="n">
+      <c r="B13" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E13" s="1" t="n">
         <v>0.470787037037037</v>
       </c>
       <c r="F13" s="0" t="n">
@@ -536,16 +537,16 @@
       <c r="A14" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C14" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D14" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E14" s="2" t="n">
+      <c r="B14" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E14" s="1" t="n">
         <v>0.470810185185185</v>
       </c>
       <c r="F14" s="0" t="n">
@@ -562,16 +563,16 @@
       <c r="A15" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C15" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D15" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E15" s="2" t="n">
+      <c r="B15" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E15" s="1" t="n">
         <v>0.470833333333333</v>
       </c>
       <c r="F15" s="0" t="n">
@@ -588,16 +589,16 @@
       <c r="A16" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C16" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D16" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E16" s="2" t="n">
+      <c r="B16" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E16" s="1" t="n">
         <v>0.470856481481482</v>
       </c>
       <c r="F16" s="0" t="n">
@@ -614,16 +615,16 @@
       <c r="A17" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C17" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D17" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E17" s="2" t="n">
+      <c r="B17" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E17" s="1" t="n">
         <v>0.47087962962963</v>
       </c>
       <c r="F17" s="0" t="n">
@@ -640,16 +641,16 @@
       <c r="A18" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C18" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D18" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E18" s="2" t="n">
+      <c r="B18" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E18" s="1" t="n">
         <v>0.470902777777778</v>
       </c>
       <c r="F18" s="0" t="n">
@@ -666,16 +667,16 @@
       <c r="A19" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C19" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D19" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E19" s="2" t="n">
+      <c r="B19" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E19" s="1" t="n">
         <v>0.470925925925926</v>
       </c>
       <c r="F19" s="0" t="n">
@@ -692,16 +693,16 @@
       <c r="A20" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C20" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D20" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E20" s="2" t="n">
+      <c r="B20" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E20" s="1" t="n">
         <v>0.470960648148148</v>
       </c>
       <c r="F20" s="0" t="n">
@@ -718,16 +719,16 @@
       <c r="A21" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C21" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D21" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E21" s="2" t="n">
+      <c r="B21" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E21" s="1" t="n">
         <v>0.470983796296296</v>
       </c>
       <c r="F21" s="0" t="n">
@@ -744,16 +745,16 @@
       <c r="A22" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C22" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D22" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E22" s="2" t="n">
+      <c r="B22" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E22" s="1" t="n">
         <v>0.471006944444444</v>
       </c>
       <c r="F22" s="0" t="n">
@@ -770,16 +771,16 @@
       <c r="A23" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C23" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D23" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E23" s="2" t="n">
+      <c r="B23" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E23" s="1" t="n">
         <v>0.471030092592593</v>
       </c>
       <c r="F23" s="0" t="n">
@@ -796,16 +797,16 @@
       <c r="A24" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C24" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D24" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E24" s="2" t="n">
+      <c r="B24" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D24" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E24" s="1" t="n">
         <v>0.471053240740741</v>
       </c>
       <c r="F24" s="0" t="n">
@@ -822,16 +823,16 @@
       <c r="A25" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C25" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D25" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E25" s="2" t="n">
+      <c r="B25" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D25" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E25" s="1" t="n">
         <v>0.471076388888889</v>
       </c>
       <c r="F25" s="0" t="n">
@@ -848,16 +849,16 @@
       <c r="A26" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C26" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D26" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E26" s="2" t="n">
+      <c r="B26" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E26" s="1" t="n">
         <v>0.471099537037037</v>
       </c>
       <c r="F26" s="0" t="n">
@@ -874,16 +875,16 @@
       <c r="A27" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C27" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D27" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E27" s="2" t="n">
+      <c r="B27" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E27" s="1" t="n">
         <v>0.471122685185185</v>
       </c>
       <c r="F27" s="0" t="n">
@@ -900,16 +901,16 @@
       <c r="A28" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C28" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D28" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E28" s="2" t="n">
+      <c r="B28" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E28" s="1" t="n">
         <v>0.471157407407407</v>
       </c>
       <c r="F28" s="0" t="n">
@@ -926,16 +927,16 @@
       <c r="A29" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C29" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D29" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E29" s="2" t="n">
+      <c r="B29" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E29" s="1" t="n">
         <v>0.471180555555556</v>
       </c>
       <c r="F29" s="0" t="n">
@@ -952,16 +953,16 @@
       <c r="A30" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C30" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D30" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E30" s="2" t="n">
+      <c r="B30" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E30" s="1" t="n">
         <v>0.471203703703704</v>
       </c>
       <c r="F30" s="0" t="n">
@@ -978,16 +979,16 @@
       <c r="A31" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="C31" s="2" t="n">
-        <v>0.470509259259259</v>
-      </c>
-      <c r="D31" s="1" t="n">
-        <v>44236</v>
-      </c>
-      <c r="E31" s="2" t="n">
+      <c r="B31" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>0.470509259259259</v>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="E31" s="1" t="n">
         <v>0.471226851851852</v>
       </c>
       <c r="F31" s="0" t="n">

</xml_diff>